<commit_message>
Created a method to log request and response to extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7210" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="7210"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>world</t>
+  </si>
+  <si>
+    <t>postProductByReadingRequestFromFile</t>
+  </si>
+  <si>
+    <t>Post a new product by reading from a json file</t>
+  </si>
+  <si>
+    <t>checking</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,7 +518,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -526,7 +535,7 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
@@ -566,6 +575,23 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -576,15 +602,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.54296875" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
@@ -756,7 +782,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -802,7 +828,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -818,6 +844,29 @@
       </c>
       <c r="G10" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>